<commit_message>
update audp sandbox3 permission
</commit_message>
<xml_diff>
--- a/role_permission_files/sandbox3_role_permission_v0.18.xlsx
+++ b/role_permission_files/sandbox3_role_permission_v0.18.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.tam\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.Outlook\17RCWJ4Y\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liang.wang\AppData\Roaming\Skype\My Skype Received Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="193">
   <si>
     <t>approve</t>
   </si>
@@ -613,25 +613,10 @@
     <t>Split reset in audit portal's reset_game_meter into reset_by_game and reset)by_terminal</t>
   </si>
   <si>
-    <t>list_reset_game_meter</t>
-  </si>
-  <si>
-    <t>reset_by_game</t>
-  </si>
-  <si>
-    <t>reset_by_terminal</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>reset_gaming_meter_log</t>
-  </si>
-  <si>
-    <t>list_reset_jackpot_meter</t>
-  </si>
-  <si>
-    <t>reset_jackpot_meter_log</t>
+    <t>reset_game</t>
+  </si>
+  <si>
+    <t>reset_terminal</t>
   </si>
 </sst>
 </file>
@@ -642,7 +627,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -650,28 +635,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -723,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -812,6 +797,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1099,7 +1087,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="8" customWidth="1"/>
@@ -1108,7 +1096,7 @@
     <col min="9" max="9" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C2" s="34" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1169,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>136</v>
       </c>
@@ -1195,7 +1183,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>139</v>
       </c>
@@ -1275,7 +1263,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>172</v>
       </c>
@@ -1289,7 +1277,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>173</v>
       </c>
@@ -1303,7 +1291,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>175</v>
       </c>
@@ -1317,7 +1305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>178</v>
       </c>
@@ -1351,7 +1339,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>189</v>
       </c>
@@ -1573,7 +1561,7 @@
       <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="8" customWidth="1"/>
@@ -2990,7 +2978,7 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" style="18" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="18" customWidth="1"/>
@@ -3369,7 +3357,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="11" customWidth="1"/>
     <col min="2" max="2" width="19.140625" style="11" customWidth="1"/>
@@ -3478,7 +3466,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="11" customWidth="1"/>
@@ -3835,11 +3823,11 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="16" customWidth="1"/>
@@ -4463,11 +4451,11 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="8" customWidth="1"/>
@@ -4532,10 +4520,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="35" t="s">
         <v>89</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -4558,10 +4546,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="35" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -4587,10 +4575,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="35" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4616,10 +4604,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="35" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -4645,33 +4633,33 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="35" t="s">
         <v>107</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4687,10 +4675,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="35" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="33" t="s">
@@ -4706,11 +4694,11 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>195</v>
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>107</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>103</v>
@@ -4729,11 +4717,11 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>196</v>
+      <c r="B11" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>103</v>
@@ -4752,10 +4740,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="35" t="s">
         <v>109</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -4769,11 +4757,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>197</v>
+      <c r="B13" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>103</v>
@@ -4805,7 +4793,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="8" bestFit="1" customWidth="1"/>

</xml_diff>